<commit_message>
Implementación Caso de Prueba Registro de Usuario
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linamfernandezg/Universidad/Calidad y Pruebas Software/3Corte/InstallationProject/Project/USB_STORE_V1/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA7E5CF-64F6-9949-A7B8-1336B07BA18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE78A92-9D4F-9845-AD03-66902CFAEBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32280" yWindow="640" windowWidth="28040" windowHeight="17440" xr2:uid="{011F8EAC-1A4B-8D49-9D4A-71DADABCE0A8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>first name</t>
   </si>
@@ -98,6 +98,147 @@
   </si>
   <si>
     <t>AnaR!2025</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Ramírez</t>
+  </si>
+  <si>
+    <t>diego.ramirez91@example.com</t>
+  </si>
+  <si>
+    <t>Dieg0!Test</t>
+  </si>
+  <si>
+    <t>Mariana</t>
+  </si>
+  <si>
+    <t>Torres</t>
+  </si>
+  <si>
+    <t>mariana.torres88@example.com</t>
+  </si>
+  <si>
+    <t>Mari#2025</t>
+  </si>
+  <si>
+    <t>Felipe</t>
+  </si>
+  <si>
+    <t>Rodríguez</t>
+  </si>
+  <si>
+    <t>f.rodriguez@example.com</t>
+  </si>
+  <si>
+    <t>FeliPass_88</t>
+  </si>
+  <si>
+    <t>Camila</t>
+  </si>
+  <si>
+    <t>Herrera</t>
+  </si>
+  <si>
+    <t>camila.h@example.com</t>
+  </si>
+  <si>
+    <t>CamH#321</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Andrés</t>
+  </si>
+  <si>
+    <t>Martínez</t>
+  </si>
+  <si>
+    <t>andres.mtz@example.com</t>
+  </si>
+  <si>
+    <t>AndMart2025!</t>
+  </si>
+  <si>
+    <t>Valentina</t>
+  </si>
+  <si>
+    <t>Salazar</t>
+  </si>
+  <si>
+    <t>v.salazar@example.com</t>
+  </si>
+  <si>
+    <t>ValeTest#1</t>
+  </si>
+  <si>
+    <t>Tomás</t>
+  </si>
+  <si>
+    <t>Ortega</t>
+  </si>
+  <si>
+    <t>tomas.ortega@example.com</t>
+  </si>
+  <si>
+    <t>3004455667</t>
+  </si>
+  <si>
+    <t>T0mPass!23</t>
+  </si>
+  <si>
+    <t>Juliana</t>
+  </si>
+  <si>
+    <t>Núñez</t>
+  </si>
+  <si>
+    <t>juliana.nunez@example.com</t>
+  </si>
+  <si>
+    <t>3112233445</t>
+  </si>
+  <si>
+    <t>Juli_Nz2025</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>Pérez</t>
+  </si>
+  <si>
+    <t>samuel.perez@example.com</t>
+  </si>
+  <si>
+    <t>3185566770</t>
+  </si>
+  <si>
+    <t>SamP!2024</t>
+  </si>
+  <si>
+    <t>Daniela</t>
+  </si>
+  <si>
+    <t>Morales</t>
+  </si>
+  <si>
+    <t>daniela.morales@example.com</t>
+  </si>
+  <si>
+    <t>3213344556</t>
+  </si>
+  <si>
+    <t>D@Morales88</t>
   </si>
 </sst>
 </file>
@@ -456,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B4BFD5-D818-4C4A-9F36-03996FBDD7E3}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,7 +609,7 @@
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,8 +631,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -513,8 +657,11 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -536,8 +683,11 @@
       <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -558,6 +708,269 @@
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3012233445</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3109876543</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3123344556</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3135566778</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3147788990</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3056677889</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementación Escritura de Resultados en Excel y Correción del Xpath para botón 'Add to Cart'
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linamfernandezg/Universidad/Calidad y Pruebas Software/3Corte/InstallationProject/Project/USB_STORE_V1/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE78A92-9D4F-9845-AD03-66902CFAEBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5940212B-16CF-B743-8A8B-B278AA7317A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32280" yWindow="640" windowWidth="28040" windowHeight="17440" xr2:uid="{011F8EAC-1A4B-8D49-9D4A-71DADABCE0A8}"/>
+    <workbookView xWindow="-38400" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{011F8EAC-1A4B-8D49-9D4A-71DADABCE0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="UsuariosRegistro" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
   <si>
     <t>first name</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>D@Morales88</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,7 +765,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Implementación de prueba End to End y Refactorización de Test
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linamfernandezg/Universidad/Calidad y Pruebas Software/3Corte/InstallationProject/Project/USB_STORE_V1/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5940212B-16CF-B743-8A8B-B278AA7317A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86D466D-EF45-374C-BDA4-D488DD46A4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{011F8EAC-1A4B-8D49-9D4A-71DADABCE0A8}"/>
+    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{011F8EAC-1A4B-8D49-9D4A-71DADABCE0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="UsuariosRegistro" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>first name</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -600,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B4BFD5-D818-4C4A-9F36-03996FBDD7E3}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,7 +615,7 @@
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,8 +640,11 @@
       <c r="H1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -663,8 +669,11 @@
       <c r="H2" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -689,8 +698,11 @@
       <c r="H3" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -715,8 +727,11 @@
       <c r="H4" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -741,8 +756,11 @@
       <c r="H5" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -767,8 +785,11 @@
       <c r="H6" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -791,10 +812,13 @@
         <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -817,10 +841,13 @@
         <v>16</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -845,8 +872,11 @@
       <c r="H9" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -871,8 +901,11 @@
       <c r="H10" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
@@ -897,8 +930,11 @@
       <c r="H11" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -923,8 +959,11 @@
       <c r="H12" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -949,8 +988,11 @@
       <c r="H13" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
@@ -974,6 +1016,9 @@
       </c>
       <c r="H14" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="I14">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adición Inicio Sesion en prueba End to End y nuevos usuarios en inputData.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linamfernandezg/Universidad/Calidad y Pruebas Software/3Corte/InstallationProject/Project/USB_STORE_V1/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86D466D-EF45-374C-BDA4-D488DD46A4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0186E570-29B6-FC49-A75C-8625A5AC1D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{011F8EAC-1A4B-8D49-9D4A-71DADABCE0A8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="217">
   <si>
     <t>first name</t>
   </si>
@@ -245,6 +245,447 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>gabriel.ríos1@example.com</t>
+  </si>
+  <si>
+    <t>3000000001</t>
+  </si>
+  <si>
+    <t>Gab#1Test</t>
+  </si>
+  <si>
+    <t>Emilia</t>
+  </si>
+  <si>
+    <t>Guzmán</t>
+  </si>
+  <si>
+    <t>emilia.guzmán2@example.com</t>
+  </si>
+  <si>
+    <t>3000000002</t>
+  </si>
+  <si>
+    <t>Emi#2Test</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Salas</t>
+  </si>
+  <si>
+    <t>daniel.salas3@example.com</t>
+  </si>
+  <si>
+    <t>3000000003</t>
+  </si>
+  <si>
+    <t>Dan#3Test</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>Castaño</t>
+  </si>
+  <si>
+    <t>paula.castaño4@example.com</t>
+  </si>
+  <si>
+    <t>3000000004</t>
+  </si>
+  <si>
+    <t>Pau#4Test</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>León</t>
+  </si>
+  <si>
+    <t>bruno.león5@example.com</t>
+  </si>
+  <si>
+    <t>3000000005</t>
+  </si>
+  <si>
+    <t>Bru#5Test</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Navarro</t>
+  </si>
+  <si>
+    <t>emma.navarro6@example.com</t>
+  </si>
+  <si>
+    <t>3000000006</t>
+  </si>
+  <si>
+    <t>Emm#6Test</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Cano</t>
+  </si>
+  <si>
+    <t>santiago.cano7@example.com</t>
+  </si>
+  <si>
+    <t>3000000007</t>
+  </si>
+  <si>
+    <t>San#7Test</t>
+  </si>
+  <si>
+    <t>Renata</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>renata.ruiz8@example.com</t>
+  </si>
+  <si>
+    <t>3000000008</t>
+  </si>
+  <si>
+    <t>Ren#8Test</t>
+  </si>
+  <si>
+    <t>Agustín</t>
+  </si>
+  <si>
+    <t>Peña</t>
+  </si>
+  <si>
+    <t>agustín.peña9@example.com</t>
+  </si>
+  <si>
+    <t>3000000009</t>
+  </si>
+  <si>
+    <t>Agu#9Test</t>
+  </si>
+  <si>
+    <t>Valeria</t>
+  </si>
+  <si>
+    <t>valeria.torres10@example.com</t>
+  </si>
+  <si>
+    <t>3000000010</t>
+  </si>
+  <si>
+    <t>Val#10Test</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Romero</t>
+  </si>
+  <si>
+    <t>lucas.romero11@example.com</t>
+  </si>
+  <si>
+    <t>3000000011</t>
+  </si>
+  <si>
+    <t>Luc#11Test</t>
+  </si>
+  <si>
+    <t>Isidora</t>
+  </si>
+  <si>
+    <t>Paz</t>
+  </si>
+  <si>
+    <t>isidora.paz12@example.com</t>
+  </si>
+  <si>
+    <t>3000000012</t>
+  </si>
+  <si>
+    <t>Isi#12Test</t>
+  </si>
+  <si>
+    <t>Martín</t>
+  </si>
+  <si>
+    <t>Soto</t>
+  </si>
+  <si>
+    <t>martín.soto13@example.com</t>
+  </si>
+  <si>
+    <t>3000000013</t>
+  </si>
+  <si>
+    <t>Mar#13Test</t>
+  </si>
+  <si>
+    <t>Bianca</t>
+  </si>
+  <si>
+    <t>Correa</t>
+  </si>
+  <si>
+    <t>bianca.correa14@example.com</t>
+  </si>
+  <si>
+    <t>3000000014</t>
+  </si>
+  <si>
+    <t>Bia#14Test</t>
+  </si>
+  <si>
+    <t>Thiago</t>
+  </si>
+  <si>
+    <t>Fuentes</t>
+  </si>
+  <si>
+    <t>thiago.fuentes15@example.com</t>
+  </si>
+  <si>
+    <t>3000000015</t>
+  </si>
+  <si>
+    <t>Thi#15Test</t>
+  </si>
+  <si>
+    <t>Antonia</t>
+  </si>
+  <si>
+    <t>Vega</t>
+  </si>
+  <si>
+    <t>antonia.vega16@example.com</t>
+  </si>
+  <si>
+    <t>3000000016</t>
+  </si>
+  <si>
+    <t>Ant#16Test</t>
+  </si>
+  <si>
+    <t>Benjamín</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>benjamín.miranda17@example.com</t>
+  </si>
+  <si>
+    <t>3000000017</t>
+  </si>
+  <si>
+    <t>Ben#17Test</t>
+  </si>
+  <si>
+    <t>Josefa</t>
+  </si>
+  <si>
+    <t>Lagos</t>
+  </si>
+  <si>
+    <t>josefa.lagos18@example.com</t>
+  </si>
+  <si>
+    <t>3000000018</t>
+  </si>
+  <si>
+    <t>Jos#18Test</t>
+  </si>
+  <si>
+    <t>Damián</t>
+  </si>
+  <si>
+    <t>Riquelme</t>
+  </si>
+  <si>
+    <t>damián.riquelme19@example.com</t>
+  </si>
+  <si>
+    <t>3000000019</t>
+  </si>
+  <si>
+    <t>Dam#19Test</t>
+  </si>
+  <si>
+    <t>Paredes</t>
+  </si>
+  <si>
+    <t>camila.paredes20@example.com</t>
+  </si>
+  <si>
+    <t>3000000020</t>
+  </si>
+  <si>
+    <t>Cam#20Test</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Muñoz</t>
+  </si>
+  <si>
+    <t>alejandro.muñoz21@example.com</t>
+  </si>
+  <si>
+    <t>3000000021</t>
+  </si>
+  <si>
+    <t>Ale#21Test</t>
+  </si>
+  <si>
+    <t>Florencia</t>
+  </si>
+  <si>
+    <t>Gallardo</t>
+  </si>
+  <si>
+    <t>florencia.gallardo22@example.com</t>
+  </si>
+  <si>
+    <t>3000000022</t>
+  </si>
+  <si>
+    <t>Flo#22Test</t>
+  </si>
+  <si>
+    <t>Axel</t>
+  </si>
+  <si>
+    <t>Salinas</t>
+  </si>
+  <si>
+    <t>axel.salinas23@example.com</t>
+  </si>
+  <si>
+    <t>3000000023</t>
+  </si>
+  <si>
+    <t>Axe#23Test</t>
+  </si>
+  <si>
+    <t>Catalina</t>
+  </si>
+  <si>
+    <t>Del Valle</t>
+  </si>
+  <si>
+    <t>catalina.del valle24@example.com</t>
+  </si>
+  <si>
+    <t>3000000024</t>
+  </si>
+  <si>
+    <t>Cat#24Test</t>
+  </si>
+  <si>
+    <t>Iván</t>
+  </si>
+  <si>
+    <t>Navarrete</t>
+  </si>
+  <si>
+    <t>iván.navarrete25@example.com</t>
+  </si>
+  <si>
+    <t>3000000025</t>
+  </si>
+  <si>
+    <t>Ivá#25Test</t>
+  </si>
+  <si>
+    <t>Amelia</t>
+  </si>
+  <si>
+    <t>Zúñiga</t>
+  </si>
+  <si>
+    <t>amelia.zúñiga26@example.com</t>
+  </si>
+  <si>
+    <t>3000000026</t>
+  </si>
+  <si>
+    <t>Ame#26Test</t>
+  </si>
+  <si>
+    <t>Maximiliano</t>
+  </si>
+  <si>
+    <t>Olivares</t>
+  </si>
+  <si>
+    <t>maximiliano.olivares27@example.com</t>
+  </si>
+  <si>
+    <t>3000000027</t>
+  </si>
+  <si>
+    <t>Max#27Test</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Palma</t>
+  </si>
+  <si>
+    <t>jose.palma28@example.com</t>
+  </si>
+  <si>
+    <t>3000000028</t>
+  </si>
+  <si>
+    <t>Jos#28Test</t>
+  </si>
+  <si>
+    <t>Nicole</t>
+  </si>
+  <si>
+    <t>Saavedra</t>
+  </si>
+  <si>
+    <t>nicole.saavedra29@example.com</t>
+  </si>
+  <si>
+    <t>3000000029</t>
+  </si>
+  <si>
+    <t>Nic#29Test</t>
+  </si>
+  <si>
+    <t>Cristóbal</t>
+  </si>
+  <si>
+    <t>Ahumada</t>
+  </si>
+  <si>
+    <t>cristóbal.ahumada30@example.com</t>
+  </si>
+  <si>
+    <t>3000000030</t>
+  </si>
+  <si>
+    <t>Cri#30Test</t>
   </si>
 </sst>
 </file>
@@ -266,12 +707,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -286,9 +733,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8B4BFD5-D818-4C4A-9F36-03996FBDD7E3}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,263 +1094,263 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>3114567890</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>3209988776</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>3181234567</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>3012233445</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>3109876543</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>3123344556</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>3135566778</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>3147788990</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9">
+      <c r="H9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>3056677889</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10">
+      <c r="H10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="3">
         <v>8</v>
       </c>
     </row>
@@ -1019,6 +1468,876 @@
       </c>
       <c r="I14">
         <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I44">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatización busqueda de datos de usuario no usados para el registro
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linamfernandezg/Universidad/Calidad y Pruebas Software/3Corte/InstallationProject/Project/USB_STORE_V1/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40096B61-F95C-134F-9F66-7BF889471156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E371FBA-B96D-9240-9D37-EECD2DA43308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="19540" xr2:uid="{011F8EAC-1A4B-8D49-9D4A-71DADABCE0A8}"/>
   </bookViews>
@@ -1055,7 +1055,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:I12"/>
+      <selection activeCell="A14" sqref="A14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1413,60 +1413,60 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13">
+      <c r="H13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14">
+      <c r="H14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="3">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización Archivos de Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linamfernandezg/Universidad/Calidad y Pruebas Software/3Corte/InstallationProject/Project/USB_STORE_V1/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB651D4-9817-3845-888D-BDA3849DE4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E7360A-EBBF-B045-9B4A-EF6E00E99FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="19540" xr2:uid="{011F8EAC-1A4B-8D49-9D4A-71DADABCE0A8}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{011F8EAC-1A4B-8D49-9D4A-71DADABCE0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="UsuariosRegistro" sheetId="1" r:id="rId1"/>
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:I15"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1534,7 +1534,7 @@
         <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="I16">
         <v>14</v>

</xml_diff>